<commit_message>
Generic Scripts Changes 23 oct
</commit_message>
<xml_diff>
--- a/locators-updated.xlsx
+++ b/locators-updated.xlsx
@@ -1503,7 +1503,7 @@
         <v>css</v>
       </c>
       <c r="C2" t="str">
-        <v>input[placeholder='Mobile Number']</v>
+        <v>input[placeholder="Mobile Number"]</v>
       </c>
       <c r="D2" t="str">
         <v>{"name":"WrongMobile Field"}</v>
@@ -1512,10 +1512,10 @@
         <v>0</v>
       </c>
       <c r="F2" t="str">
-        <v>input[placeholder='Mobile Number']</v>
+        <v>input[placeholder="Mobile Number"]</v>
       </c>
       <c r="G2" t="str">
-        <v>2025-10-20T05:01:28.767Z</v>
+        <v>2025-10-22T04:02:10.596Z</v>
       </c>
     </row>
     <row r="3">
@@ -1538,7 +1538,7 @@
         <v>input[placeholder='Enter Password']</v>
       </c>
       <c r="G3" t="str">
-        <v>2025-10-20T05:01:28.767Z</v>
+        <v>2025-10-22T04:02:10.597Z</v>
       </c>
     </row>
     <row r="4">

</xml_diff>